<commit_message>
changing keyword StoreValueIn and StoreTextIn
Changed StoredValueIn and StoreTextIn to PutValueIn and PutTextIn. Usage
in KeywordDrivenTest should be {{get.<name>}}. Adding sample usage of
keywords xls file.
</commit_message>
<xml_diff>
--- a/doc/Keywords.xlsx
+++ b/doc/Keywords.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Waits" sheetId="2" r:id="rId2"/>
     <sheet name="Assertions &amp; Verifications" sheetId="3" r:id="rId3"/>
     <sheet name="If Conditions" sheetId="4" r:id="rId4"/>
-    <sheet name="Store" sheetId="5" r:id="rId5"/>
+    <sheet name="Put" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -255,12 +255,6 @@
     <t>Clears and sets value of an input field.</t>
   </si>
   <si>
-    <t>StoreValueIn</t>
-  </si>
-  <si>
-    <t>StoreTextIn</t>
-  </si>
-  <si>
     <t>Clicks on a link, button, checkbox or radio button.</t>
   </si>
   <si>
@@ -569,13 +563,19 @@
   </si>
   <si>
     <t>SelectByText</t>
+  </si>
+  <si>
+    <t>PutValueIn</t>
+  </si>
+  <si>
+    <t>PutTextIn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -729,6 +729,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -763,6 +764,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -938,21 +940,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="37" style="4" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -963,7 +965,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -974,7 +976,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -985,7 +987,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -996,7 +998,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1007,7 +1009,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1015,10 +1017,10 @@
         <v>76</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1026,238 +1028,238 @@
         <v>77</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="105">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="60">
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="60">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="60">
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="60">
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="60">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="60">
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="60">
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="75">
+    <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="75">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" ht="45">
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" ht="30">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" ht="30">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" ht="30">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1268,21 +1270,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="50.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1293,176 +1295,176 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1471,21 +1473,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1496,235 +1498,235 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30">
-      <c r="A5" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30">
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="60">
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30">
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1734,21 +1736,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="2" width="44.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1759,109 +1761,109 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30">
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="45">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -1871,21 +1873,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1896,26 +1898,26 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>174</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="60">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>175</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting changes w.r.t new version. can find comments in change log.
</commit_message>
<xml_diff>
--- a/doc/Keywords.xlsx
+++ b/doc/Keywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="178">
   <si>
     <t>Get</t>
   </si>
@@ -569,6 +569,12 @@
   </si>
   <si>
     <t>PutTextIn</t>
+  </si>
+  <si>
+    <t>AssertNotSelectOptions</t>
+  </si>
+  <si>
+    <t>AssertNotAttribute</t>
   </si>
 </sst>
 </file>
@@ -943,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1474,9 +1480,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1599,133 +1605,155 @@
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>49</v>
+        <v>176</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>110</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commiting changes w.r.t new version
</commit_message>
<xml_diff>
--- a/doc/Keywords.xlsx
+++ b/doc/Keywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
   <si>
     <t>Get</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>Wait</t>
-  </si>
-  <si>
-    <t>WaitForPageToLoad</t>
   </si>
   <si>
     <t>WaitForElementPresent</t>
@@ -496,9 +493,6 @@
   </si>
   <si>
     <t>Sleeps execution for the specified time.</t>
-  </si>
-  <si>
-    <t>Waits for a new page to load.</t>
   </si>
   <si>
     <t>Waits for the specified element to be present on the page.</t>
@@ -949,7 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -965,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,296 +970,296 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1277,7 +1271,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1295,10 +1289,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1306,30 +1300,32 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1340,7 +1336,7 @@
         <v>154</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1348,10 +1344,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1359,10 +1355,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1370,10 +1366,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1381,10 +1377,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1392,10 +1388,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1406,7 +1402,7 @@
         <v>162</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1414,7 +1410,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>147</v>
@@ -1425,52 +1421,41 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>170</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1498,263 +1483,263 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1783,115 +1768,115 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -1920,32 +1905,32 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed android support and updated keywords
</commit_message>
<xml_diff>
--- a/doc/Keywords.xlsx
+++ b/doc/Keywords.xlsx
@@ -4,21 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
     <sheet name="Waits" sheetId="2" r:id="rId2"/>
     <sheet name="Assertions &amp; Verifications" sheetId="3" r:id="rId3"/>
     <sheet name="If Conditions" sheetId="4" r:id="rId4"/>
-    <sheet name="Put" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="170">
   <si>
     <t>Get</t>
   </si>
@@ -266,14 +265,6 @@
   </si>
   <si>
     <t>Uncheck a toggle-button (checkbox)</t>
-  </si>
-  <si>
-    <t>locator - an element locator
-value - element value will be stored in</t>
-  </si>
-  <si>
-    <t>locator - an element locator
-value - element text will be stored in</t>
   </si>
   <si>
     <t>locator - an element locator
@@ -288,12 +279,6 @@
 value - the value to type.(random number will be appended to the value at run time.)</t>
   </si>
   <si>
-    <t>Stores the text of the element. This keyword must not be overridden in your keyword class.</t>
-  </si>
-  <si>
-    <t>Stores the value of the element. This keyword must not be overridden in your keyword class.</t>
-  </si>
-  <si>
     <t>Move the focus to the specified element; for example, if the element is an input field, move the cursor to that field.</t>
   </si>
   <si>
@@ -557,12 +542,6 @@
   </si>
   <si>
     <t>SelectByText</t>
-  </si>
-  <si>
-    <t>PutValueIn</t>
-  </si>
-  <si>
-    <t>PutTextIn</t>
   </si>
   <si>
     <t>AssertNotSelectOptions</t>
@@ -943,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1017,7 +996,7 @@
         <v>75</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1028,7 +1007,7 @@
         <v>76</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -1036,10 +1015,10 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1099,13 +1078,13 @@
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -1113,7 +1092,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>74</v>
@@ -1124,7 +1103,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>78</v>
@@ -1135,7 +1114,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>74</v>
@@ -1146,7 +1125,7 @@
         <v>30</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>78</v>
@@ -1157,7 +1136,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>74</v>
@@ -1168,7 +1147,7 @@
         <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>78</v>
@@ -1179,7 +1158,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>74</v>
@@ -1190,7 +1169,7 @@
         <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>74</v>
@@ -1201,10 +1180,10 @@
         <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -1212,10 +1191,10 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,7 +1202,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1232,7 +1211,7 @@
         <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -1241,7 +1220,7 @@
         <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -1250,7 +1229,7 @@
         <v>40</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -1259,7 +1238,7 @@
         <v>42</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1273,7 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1300,10 +1279,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1311,10 +1290,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1322,10 +1301,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1333,10 +1312,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1344,10 +1323,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1355,10 +1334,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1366,10 +1345,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1377,10 +1356,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1388,10 +1367,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1399,10 +1378,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1410,10 +1389,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1421,10 +1400,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,7 +1411,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C14" s="3"/>
     </row>
@@ -1441,10 +1420,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1452,10 +1431,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1467,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1494,21 +1473,21 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1516,21 +1495,21 @@
         <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1538,7 +1517,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>74</v>
@@ -1549,7 +1528,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>74</v>
@@ -1560,7 +1539,7 @@
         <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>74</v>
@@ -1571,7 +1550,7 @@
         <v>51</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>74</v>
@@ -1582,21 +1561,21 @@
         <v>47</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1604,10 +1583,10 @@
         <v>48</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1615,7 +1594,7 @@
         <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>74</v>
@@ -1626,7 +1605,7 @@
         <v>54</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>74</v>
@@ -1637,29 +1616,29 @@
         <v>50</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>74</v>
@@ -1670,7 +1649,7 @@
         <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>74</v>
@@ -1681,21 +1660,21 @@
         <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1703,10 +1682,10 @@
         <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1714,10 +1693,10 @@
         <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1725,10 +1704,10 @@
         <v>58</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1736,10 +1715,10 @@
         <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1779,7 +1758,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>74</v>
@@ -1790,7 +1769,7 @@
         <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>74</v>
@@ -1801,7 +1780,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>74</v>
@@ -1812,7 +1791,7 @@
         <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>74</v>
@@ -1823,10 +1802,10 @@
         <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1834,10 +1813,10 @@
         <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1845,10 +1824,10 @@
         <v>66</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1856,82 +1835,29 @@
         <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C11" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>83</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhancements, fixes and updated docs for the upcomming release
</commit_message>
<xml_diff>
--- a/doc/Keywords.xlsx
+++ b/doc/Keywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="167">
   <si>
     <t>Get</t>
   </si>
@@ -58,9 +58,6 @@
     <t>WaitForNotText</t>
   </si>
   <si>
-    <t>WaitForAlert</t>
-  </si>
-  <si>
     <t>WaitForAlertPresent</t>
   </si>
   <si>
@@ -77,12 +74,6 @@
   </si>
   <si>
     <t>ClearAndType</t>
-  </si>
-  <si>
-    <t>TypeUnique</t>
-  </si>
-  <si>
-    <t>ClearAndTypeUnique</t>
   </si>
   <si>
     <t>TypeDate</t>
@@ -492,9 +483,6 @@
     <t>Waits for the specified element to be visible.</t>
   </si>
   <si>
-    <t>Waits for an alert to be present with the specified text.</t>
-  </si>
-  <si>
     <t>Waits for an alert to be present.</t>
   </si>
   <si>
@@ -532,9 +520,6 @@
     <t>value - page title to appear.</t>
   </si>
   <si>
-    <t>value - alert text to appear.</t>
-  </si>
-  <si>
     <t>value - frame id to appear.</t>
   </si>
   <si>
@@ -548,6 +533,12 @@
   </si>
   <si>
     <t>AssertNotAttribute</t>
+  </si>
+  <si>
+    <t>TypeRandomAlphabets</t>
+  </si>
+  <si>
+    <t>ClearAndTypeRandomAlphabets</t>
   </si>
 </sst>
 </file>
@@ -922,13 +913,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" style="4" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -938,10 +929,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -949,296 +940,296 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>165</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1250,10 +1241,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,10 +1259,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,10 +1270,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1290,10 +1281,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1301,10 +1292,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1312,10 +1303,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1323,10 +1314,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1334,10 +1325,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1345,10 +1336,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1356,10 +1347,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1367,10 +1358,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1378,10 +1369,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1389,52 +1380,41 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>164</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1446,7 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1462,263 +1442,263 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1747,115 +1727,115 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C11" s="2"/>
     </row>

</xml_diff>